<commit_message>
test cases to show logging
</commit_message>
<xml_diff>
--- a/test/model-rule-data/fetch_relations.xlsx
+++ b/test/model-rule-data/fetch_relations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>fetch_relation</t>
   </si>
@@ -41,16 +41,16 @@
     <t>U</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>customer name</t>
   </si>
   <si>
-    <t>foo</t>
-  </si>
-  <si>
-    <t>cust.amount.value</t>
+    <t>"foo"</t>
+  </si>
+  <si>
+    <t>gate</t>
+  </si>
+  <si>
+    <t>variable</t>
   </si>
 </sst>
 </file>
@@ -368,17 +368,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D5"/>
+  <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
@@ -388,35 +388,43 @@
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>1</v>
+      <c r="B5" t="s">
+        <v>4</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>